<commit_message>
Point To The Correct JMX Files -> Dog API Run JMX Files
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Dog API JMX Files.xlsx
+++ b/src/test/resources/data/Dog API JMX Files.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{D533DA6B-E2ED-401F-8856-0ED26E605460}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7DE28A9E-370F-457B-B1F9-8A3D22234E43}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{D533DA6B-E2ED-401F-8856-0ED26E605460}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7FEFFF50-4DAA-48AF-88F3-D21590DEA9EA}"/>
   <bookViews>
     <workbookView xWindow="-3375" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,13 +77,13 @@
     <t>Is Project Path</t>
   </si>
   <si>
-    <t>Dog API JMX Files.xlsx</t>
-  </si>
-  <si>
     <t>Dog API Run JMX Files One</t>
   </si>
   <si>
     <t>Dog API Run JMX Files Two</t>
+  </si>
+  <si>
+    <t>Dog API Test.jmx</t>
   </si>
 </sst>
 </file>
@@ -414,7 +414,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,13 +440,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
         <v>15</v>
@@ -454,13 +454,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
         <v>15</v>

</xml_diff>